<commit_message>
Added PDF Concept Document and Powerpoint
</commit_message>
<xml_diff>
--- a/your game name here.xlsx
+++ b/your game name here.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter.lowe\Desktop\proto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C00308099\Desktop\Concept Doc GIT\concept25-Tristan-Timmins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592968BF-B044-48C7-B482-7309AED76571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E4DADC-920B-4DA8-871C-FC2E41EF3B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{B114BF61-C9F1-47F8-B51B-C5362F104DFD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B114BF61-C9F1-47F8-B51B-C5362F104DFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -311,9 +311,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -351,7 +351,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -457,7 +457,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -599,7 +599,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -610,7 +610,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +658,7 @@
       </c>
       <c r="G2" s="2">
         <f>SUM(G4:G23)</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
         <v>2</v>
@@ -772,7 +772,9 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="6">
+        <v>25</v>
+      </c>
       <c r="E5">
         <v>25</v>
       </c>
@@ -782,7 +784,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -819,7 +821,9 @@
       <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
       <c r="E6">
         <v>5</v>
       </c>
@@ -866,7 +870,9 @@
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6">
+        <v>5</v>
+      </c>
       <c r="E7">
         <v>15</v>
       </c>
@@ -876,7 +882,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
@@ -913,7 +919,9 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="6">
+        <v>15</v>
+      </c>
       <c r="E8">
         <v>15</v>
       </c>
@@ -923,7 +931,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -1058,7 +1066,9 @@
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="6">
+        <v>5</v>
+      </c>
       <c r="E11">
         <v>20</v>
       </c>
@@ -1068,7 +1078,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -1154,7 +1164,9 @@
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="D13" s="6"/>
+      <c r="D13" s="6">
+        <v>0</v>
+      </c>
       <c r="E13">
         <v>20</v>
       </c>

</xml_diff>